<commit_message>
Greyed out empty cells in mana bonus
</commit_message>
<xml_diff>
--- a/templates/mutation_tree_template.xlsx
+++ b/templates/mutation_tree_template.xlsx
@@ -464,11 +464,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -685,819 +681,815 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15:N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="0"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="0"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="0"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="0"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="D6" s="10" t="s">
+      <c r="B6" s="7"/>
+      <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="H6" s="10" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="12" t="n">
+      <c r="I6" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="L6" s="10" t="s">
+      <c r="J6" s="10"/>
+      <c r="L6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="13"/>
-      <c r="N6" s="11"/>
-      <c r="P6" s="10" t="s">
+      <c r="M6" s="12"/>
+      <c r="N6" s="10"/>
+      <c r="P6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="T6" s="10" t="s">
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="T6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="15" t="n">
+      <c r="B7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="15" t="n">
+      <c r="J7" s="10"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="N7" s="11"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="T7" s="16" t="s">
+      <c r="N7" s="10"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="T7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="15" t="n">
+      <c r="B8" s="7"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14" t="n">
         <v>25</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="15" t="n">
+      <c r="J8" s="10"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="15" t="n">
+      <c r="N8" s="10"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="14" t="n">
         <v>120</v>
       </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="18" t="n">
+      <c r="B9" s="7"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="15" t="n">
+      <c r="F9" s="10"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="15" t="n">
+      <c r="J9" s="10"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="15" t="n">
+      <c r="N9" s="10"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="14" t="n">
         <v>60</v>
       </c>
-      <c r="R9" s="11"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="15" t="n">
+      <c r="R9" s="10"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="V9" s="11"/>
+      <c r="V9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8"/>
-      <c r="D10" s="19" t="n">
+      <c r="B10" s="7"/>
+      <c r="D10" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="H10" s="19" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="H10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="L10" s="19" t="s">
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="L10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="P10" s="19" t="s">
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="P10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="T10" s="20" t="s">
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="T10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="8"/>
-      <c r="N11" s="21"/>
+      <c r="B11" s="7"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="23"/>
+      <c r="B12" s="7"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8"/>
-      <c r="O13" s="24"/>
+      <c r="B13" s="7"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="25"/>
+      <c r="B14" s="7"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
-      <c r="D15" s="10" t="s">
+      <c r="B15" s="7"/>
+      <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="15" t="n">
+      <c r="E15" s="14" t="n">
         <v>60</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="H15" s="10" t="s">
+      <c r="F15" s="10"/>
+      <c r="H15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="15" t="n">
+      <c r="I15" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="J15" s="11"/>
-      <c r="L15" s="26" t="s">
+      <c r="J15" s="10"/>
+      <c r="L15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="15" t="n">
+      <c r="M15" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="N15" s="13"/>
-      <c r="P15" s="10" t="s">
+      <c r="N15" s="10"/>
+      <c r="P15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="13" t="n">
+      <c r="Q15" s="12" t="n">
         <v>40</v>
       </c>
-      <c r="R15" s="13" t="n">
+      <c r="R15" s="12" t="n">
         <v>110</v>
       </c>
-      <c r="T15" s="10" t="s">
+      <c r="T15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="15" t="n">
+      <c r="B16" s="7"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="15" t="n">
+      <c r="F16" s="10"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="14" t="n">
         <v>70</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="15" t="n">
+      <c r="J16" s="10"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="N16" s="13"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="13" t="n">
+      <c r="N16" s="10"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="12" t="n">
         <v>35</v>
       </c>
-      <c r="R16" s="13" t="n">
+      <c r="R16" s="12" t="n">
         <v>90</v>
       </c>
-      <c r="T16" s="10"/>
-      <c r="U16" s="15" t="n">
+      <c r="T16" s="9"/>
+      <c r="U16" s="14" t="n">
         <v>200</v>
       </c>
-      <c r="V16" s="11"/>
+      <c r="V16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="15" t="n">
+      <c r="B17" s="7"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="15" t="n">
+      <c r="F17" s="10"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="15" t="n">
+      <c r="J17" s="10"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="N17" s="13"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="13" t="n">
+      <c r="N17" s="10"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="12" t="n">
         <v>30</v>
       </c>
-      <c r="R17" s="13" t="n">
+      <c r="R17" s="12" t="n">
         <v>70</v>
       </c>
-      <c r="S17" s="17"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="15" t="n">
+      <c r="S17" s="16"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="14" t="n">
         <v>110</v>
       </c>
-      <c r="V17" s="11"/>
+      <c r="V17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="8"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="15" t="n">
+      <c r="B18" s="7"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="15" t="n">
+      <c r="F18" s="10"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="15" t="n">
+      <c r="J18" s="10"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="N18" s="13"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="15" t="n">
+      <c r="N18" s="10"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="R18" s="13" t="n">
+      <c r="R18" s="12" t="n">
         <v>55</v>
       </c>
-      <c r="T18" s="16"/>
-      <c r="U18" s="15" t="n">
+      <c r="T18" s="15"/>
+      <c r="U18" s="14" t="n">
         <v>90</v>
       </c>
-      <c r="V18" s="11"/>
+      <c r="V18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="8"/>
-      <c r="D19" s="19" t="s">
+      <c r="B19" s="7"/>
+      <c r="D19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="H19" s="19" t="s">
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="H19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="L19" s="19" t="s">
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="L19" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="P19" s="19" t="s">
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="P19" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="T19" s="27" t="n">
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="T19" s="26" t="n">
         <v>14904</v>
       </c>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="F20" s="21"/>
+      <c r="B20" s="7"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="8"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
+      <c r="B21" s="7"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="8"/>
-      <c r="G22" s="24"/>
+      <c r="B22" s="7"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="8"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="25"/>
+      <c r="B23" s="7"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="8"/>
-      <c r="H24" s="26" t="s">
+      <c r="B24" s="7"/>
+      <c r="H24" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="15" t="n">
+      <c r="I24" s="14" t="n">
         <v>80</v>
       </c>
-      <c r="J24" s="11"/>
-      <c r="L24" s="26" t="s">
+      <c r="J24" s="10"/>
+      <c r="L24" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="M24" s="15" t="n">
+      <c r="M24" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="N24" s="11"/>
-      <c r="P24" s="26" t="s">
+      <c r="N24" s="10"/>
+      <c r="P24" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="Q24" s="15" t="n">
+      <c r="Q24" s="14" t="n">
         <v>110</v>
       </c>
-      <c r="R24" s="11"/>
-      <c r="T24" s="28"/>
+      <c r="R24" s="10"/>
+      <c r="T24" s="27"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="8"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="15" t="n">
+      <c r="B25" s="7"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="J25" s="11"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="15" t="n">
+      <c r="J25" s="10"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="14" t="n">
         <v>70</v>
       </c>
-      <c r="N25" s="11"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="15" t="n">
+      <c r="N25" s="10"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="14" t="n">
         <v>80</v>
       </c>
-      <c r="R25" s="11"/>
-      <c r="T25" s="28"/>
+      <c r="R25" s="10"/>
+      <c r="T25" s="27"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="8"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="15" t="n">
+      <c r="B26" s="7"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="14" t="n">
         <v>25</v>
       </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="15" t="n">
+      <c r="J26" s="10"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="N26" s="11"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="15" t="n">
+      <c r="N26" s="10"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="R26" s="11"/>
-      <c r="T26" s="28"/>
+      <c r="R26" s="10"/>
+      <c r="T26" s="27"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="8"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="15" t="n">
+      <c r="B27" s="7"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="15" t="n">
+      <c r="J27" s="10"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="N27" s="11"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="15" t="n">
+      <c r="N27" s="10"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="R27" s="11"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
+      <c r="R27" s="10"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="8"/>
-      <c r="H28" s="19" t="s">
+      <c r="B28" s="7"/>
+      <c r="H28" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="L28" s="19" t="s">
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="L28" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="P28" s="19" t="s">
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="P28" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="8"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="25"/>
+      <c r="B29" s="7"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="24"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="8"/>
-      <c r="G30" s="24"/>
+      <c r="B30" s="7"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="8"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
+      <c r="B31" s="7"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="8"/>
-      <c r="F32" s="24"/>
+      <c r="B32" s="7"/>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="8"/>
-      <c r="D33" s="10" t="s">
+      <c r="B33" s="7"/>
+      <c r="D33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="H33" s="10" t="s">
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="H33" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="15" t="n">
+      <c r="I33" s="14" t="n">
         <v>70</v>
       </c>
-      <c r="J33" s="15" t="n">
+      <c r="J33" s="14" t="n">
         <v>200</v>
       </c>
-      <c r="L33" s="10" t="s">
+      <c r="L33" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="M33" s="15" t="n">
+      <c r="M33" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="N33" s="11"/>
-      <c r="P33" s="10" t="s">
+      <c r="N33" s="10"/>
+      <c r="P33" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="T33" s="10" t="s">
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="T33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="8"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="15" t="n">
+      <c r="B34" s="7"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="14" t="n">
         <v>55</v>
       </c>
-      <c r="J34" s="15" t="n">
+      <c r="J34" s="14" t="n">
         <v>180</v>
       </c>
-      <c r="L34" s="10"/>
-      <c r="M34" s="15" t="n">
+      <c r="L34" s="9"/>
+      <c r="M34" s="14" t="n">
         <v>80</v>
       </c>
-      <c r="N34" s="11"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="15" t="n">
+      <c r="N34" s="10"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="14" t="n">
         <v>70</v>
       </c>
-      <c r="R34" s="11"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="15" t="n">
+      <c r="R34" s="10"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="14" t="n">
         <v>70</v>
       </c>
-      <c r="V34" s="11"/>
+      <c r="V34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="8"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="15" t="n">
+      <c r="B35" s="7"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="15" t="n">
+      <c r="F35" s="10"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="J35" s="15" t="n">
+      <c r="J35" s="14" t="n">
         <v>150</v>
       </c>
-      <c r="K35" s="17"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="15" t="n">
+      <c r="K35" s="16"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="N35" s="11"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="15" t="n">
+      <c r="N35" s="10"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="R35" s="11"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="15" t="n">
+      <c r="R35" s="10"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="V35" s="11"/>
+      <c r="V35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="8"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="15" t="n">
+      <c r="B36" s="7"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="15" t="n">
+      <c r="F36" s="10"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="14" t="n">
         <v>25</v>
       </c>
-      <c r="J36" s="15" t="n">
+      <c r="J36" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="L36" s="16"/>
-      <c r="M36" s="15" t="n">
+      <c r="L36" s="15"/>
+      <c r="M36" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="N36" s="11"/>
-      <c r="P36" s="16"/>
-      <c r="Q36" s="15" t="n">
+      <c r="N36" s="10"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="R36" s="11"/>
-      <c r="T36" s="16"/>
-      <c r="U36" s="15" t="n">
+      <c r="R36" s="10"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="V36" s="11"/>
+      <c r="V36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="8"/>
-      <c r="D37" s="32" t="n">
+      <c r="B37" s="7"/>
+      <c r="D37" s="31" t="n">
         <v>100200</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="H37" s="19" t="s">
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="H37" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="L37" s="19" t="s">
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="L37" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="P37" s="19" t="s">
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="P37" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="T37" s="33" t="s">
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="T37" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="U37" s="33"/>
-      <c r="V37" s="33"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="8"/>
-      <c r="F38" s="21"/>
-      <c r="N38" s="21"/>
+      <c r="B38" s="7"/>
+      <c r="F38" s="20"/>
+      <c r="N38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="8"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="23"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="23"/>
+      <c r="B39" s="7"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="22"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="8"/>
-      <c r="G40" s="24"/>
-      <c r="O40" s="24"/>
+      <c r="B40" s="7"/>
+      <c r="G40" s="23"/>
+      <c r="O40" s="23"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="8"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="25"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="25"/>
+      <c r="B41" s="7"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="24"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="24"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="8"/>
-      <c r="H42" s="10" t="s">
+      <c r="B42" s="7"/>
+      <c r="H42" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I42" s="15" t="n">
+      <c r="I42" s="14" t="n">
         <v>70</v>
       </c>
-      <c r="J42" s="11"/>
-      <c r="L42" s="10" t="s">
+      <c r="J42" s="10"/>
+      <c r="L42" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="M42" s="15" t="n">
+      <c r="M42" s="14" t="n">
         <v>60</v>
       </c>
-      <c r="N42" s="11"/>
-      <c r="P42" s="10" t="s">
+      <c r="N42" s="10"/>
+      <c r="P42" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="T42" s="28"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="T42" s="27"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="8"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="15" t="n">
+      <c r="B43" s="7"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="J43" s="11"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="15" t="n">
+      <c r="J43" s="10"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="N43" s="11"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="15" t="n">
+      <c r="N43" s="10"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="R43" s="15" t="n">
+      <c r="R43" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="T43" s="28"/>
+      <c r="T43" s="27"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="8"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="15" t="n">
+      <c r="B44" s="7"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="14" t="n">
         <v>25</v>
       </c>
-      <c r="J44" s="11"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="16"/>
-      <c r="M44" s="15" t="n">
+      <c r="J44" s="10"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="N44" s="11"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="15" t="n">
+      <c r="N44" s="10"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="14" t="n">
         <v>40</v>
       </c>
-      <c r="R44" s="15" t="n">
+      <c r="R44" s="14" t="n">
         <v>80</v>
       </c>
-      <c r="T44" s="28"/>
+      <c r="T44" s="27"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="8"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="15" t="n">
+      <c r="B45" s="7"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="J45" s="11"/>
-      <c r="L45" s="16"/>
-      <c r="M45" s="15" t="n">
+      <c r="J45" s="10"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="14" t="n">
         <v>20</v>
       </c>
-      <c r="N45" s="11"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="15" t="n">
+      <c r="N45" s="10"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="R45" s="15" t="n">
+      <c r="R45" s="14" t="n">
         <v>60</v>
       </c>
-      <c r="T45" s="28"/>
-      <c r="U45" s="28"/>
+      <c r="T45" s="27"/>
+      <c r="U45" s="27"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="8"/>
-      <c r="H46" s="19" t="s">
+      <c r="B46" s="7"/>
+      <c r="H46" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="L46" s="19" t="s">
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="L46" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="P46" s="19" t="s">
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="P46" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="8"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="8"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="8"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="8"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="8"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="8"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="8"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="8"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="8"/>
+      <c r="B55" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="62">

</xml_diff>